<commit_message>
fix projects spreadsheet; but still issue with cell line for a specific genome
</commit_message>
<xml_diff>
--- a/data/GEP00006/20171102_GEP00006.xlsx
+++ b/data/GEP00006/20171102_GEP00006.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\core\genome_editing\data\group_folders\Projects\GE201- Narita A549 Jag1\NGS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25000" windowHeight="15220" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -21,8 +16,11 @@
     <sheet name="Plate" sheetId="7" r:id="rId7"/>
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -603,9 +601,6 @@
     <t>PCR Dilution 1:100 for indexing, temporarily stored.</t>
   </si>
   <si>
-    <t xml:space="preserve">gDNA </t>
-  </si>
-  <si>
     <t>FLD0001</t>
   </si>
   <si>
@@ -895,12 +890,15 @@
   </si>
   <si>
     <t>SLX-15109</t>
+  </si>
+  <si>
+    <t>gDNA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1036,7 +1034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1071,7 +1069,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1248,7 +1246,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1258,22 +1256,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125"/>
-    <col min="6" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" customWidth="1"/>
-    <col min="10" max="1025" width="11.5703125"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="6" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1302,7 +1297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1338,6 +1333,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1345,21 +1345,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="1025" width="11.5703125"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1391,7 +1389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1423,7 +1421,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="I9" s="1"/>
     </row>
   </sheetData>
@@ -1433,6 +1431,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1440,22 +1443,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1478,7 +1480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1501,7 +1503,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1524,21 +1526,26 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1546,20 +1553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1580,6 +1585,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1587,35 +1597,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="31.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" customWidth="1"/>
-    <col min="17" max="18" width="31.7109375" customWidth="1"/>
-    <col min="19" max="21" width="14.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" customWidth="1"/>
-    <col min="23" max="1025" width="11.5703125"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="31.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" customWidth="1"/>
+    <col min="17" max="18" width="31.6640625" customWidth="1"/>
+    <col min="19" max="21" width="14.83203125" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1668,7 +1676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1721,7 +1729,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1781,6 +1789,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1788,23 +1801,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="7" width="11.5703125"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="1025" width="11.5703125"/>
+    <col min="1" max="2" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1846,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1862,7 +1872,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1920,7 +1930,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -1949,7 +1959,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1978,7 +1988,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -2007,7 +2017,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -2065,7 +2075,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -2094,7 +2104,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2123,7 +2133,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -2152,7 +2162,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -2181,7 +2191,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -2210,7 +2220,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -2239,7 +2249,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -2268,7 +2278,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2297,7 +2307,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -2326,7 +2336,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2355,7 +2365,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2384,7 +2394,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2413,7 +2423,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2442,7 +2452,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -2471,7 +2481,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -2500,7 +2510,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2529,7 +2539,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2558,7 +2568,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2587,7 +2597,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2616,7 +2626,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2645,7 +2655,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -2674,7 +2684,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2703,7 +2713,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -2732,7 +2742,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -2761,7 +2771,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2790,7 +2800,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2819,7 +2829,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2848,7 +2858,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2877,7 +2887,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -2906,7 +2916,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2935,7 +2945,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -2964,7 +2974,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -2993,7 +3003,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -3022,7 +3032,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -3080,7 +3090,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -3109,7 +3119,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3138,7 +3148,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -3167,7 +3177,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -3196,7 +3206,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -3225,7 +3235,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -3254,7 +3264,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -3283,7 +3293,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -3312,7 +3322,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -3341,7 +3351,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -3370,7 +3380,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -3399,7 +3409,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -3428,7 +3438,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -3457,7 +3467,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -3486,7 +3496,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -3515,7 +3525,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -3544,7 +3554,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -3573,7 +3583,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -3602,7 +3612,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -3631,7 +3641,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -3660,7 +3670,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -3689,7 +3699,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -3718,7 +3728,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -3747,7 +3757,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -3776,7 +3786,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -3805,7 +3815,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -3834,7 +3844,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -3863,7 +3873,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -3892,7 +3902,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -3921,7 +3931,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3950,7 +3960,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -3979,7 +3989,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -4008,7 +4018,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -4037,7 +4047,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -4066,7 +4076,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -4095,7 +4105,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -4124,7 +4134,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -4153,7 +4163,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -4173,7 +4183,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -4193,7 +4203,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -4213,7 +4223,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -4233,7 +4243,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -4253,7 +4263,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -4273,7 +4283,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -4293,7 +4303,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -4313,7 +4323,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>82</v>
       </c>
@@ -4342,7 +4352,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>82</v>
       </c>
@@ -4371,7 +4381,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>82</v>
       </c>
@@ -4400,7 +4410,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>82</v>
       </c>
@@ -4426,7 +4436,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>82</v>
       </c>
@@ -4452,7 +4462,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>82</v>
       </c>
@@ -4478,7 +4488,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>82</v>
       </c>
@@ -4504,7 +4514,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>82</v>
       </c>
@@ -4525,6 +4535,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4532,20 +4547,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -4559,7 +4573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -4580,6 +4594,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4587,22 +4606,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -4625,7 +4643,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -4633,23 +4651,23 @@
         <v>84</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" t="s">
         <v>190</v>
-      </c>
-      <c r="D2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" t="s">
-        <v>191</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE(A2,B2)</f>
         <v>GEP00006_01A1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -4660,20 +4678,20 @@
         <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E3" t="s">
         <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G66" si="0">CONCATENATE(A3,B3)</f>
         <v>GEP00006_01B1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -4684,20 +4702,20 @@
         <v>188</v>
       </c>
       <c r="D4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E4" t="s">
         <v>187</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -4708,20 +4726,20 @@
         <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" t="s">
         <v>187</v>
       </c>
       <c r="F5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -4732,20 +4750,20 @@
         <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E6" t="s">
         <v>187</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -4756,20 +4774,20 @@
         <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E7" t="s">
         <v>187</v>
       </c>
       <c r="F7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -4780,20 +4798,20 @@
         <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E8" t="s">
         <v>187</v>
       </c>
       <c r="F8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -4804,20 +4822,20 @@
         <v>188</v>
       </c>
       <c r="D9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E9" t="s">
         <v>187</v>
       </c>
       <c r="F9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -4828,20 +4846,20 @@
         <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E10" t="s">
         <v>187</v>
       </c>
       <c r="F10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -4852,20 +4870,20 @@
         <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E11" t="s">
         <v>187</v>
       </c>
       <c r="F11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="14">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -4876,13 +4894,13 @@
         <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E12" t="s">
         <v>187</v>
       </c>
       <c r="F12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -4890,7 +4908,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -4901,20 +4919,20 @@
         <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E13" t="s">
         <v>187</v>
       </c>
       <c r="F13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -4925,20 +4943,20 @@
         <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E14" t="s">
         <v>187</v>
       </c>
       <c r="F14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -4949,20 +4967,20 @@
         <v>188</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E15" t="s">
         <v>187</v>
       </c>
       <c r="F15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -4973,20 +4991,20 @@
         <v>188</v>
       </c>
       <c r="D16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E16" t="s">
         <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -4997,20 +5015,20 @@
         <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E17" t="s">
         <v>187</v>
       </c>
       <c r="F17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -5021,20 +5039,20 @@
         <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E18" t="s">
         <v>187</v>
       </c>
       <c r="F18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -5045,20 +5063,20 @@
         <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E19" t="s">
         <v>187</v>
       </c>
       <c r="F19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -5069,20 +5087,20 @@
         <v>188</v>
       </c>
       <c r="D20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E20" t="s">
         <v>187</v>
       </c>
       <c r="F20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -5093,20 +5111,20 @@
         <v>188</v>
       </c>
       <c r="D21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E21" t="s">
         <v>187</v>
       </c>
       <c r="F21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -5117,20 +5135,20 @@
         <v>188</v>
       </c>
       <c r="D22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E22" t="s">
         <v>187</v>
       </c>
       <c r="F22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -5141,20 +5159,20 @@
         <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E23" t="s">
         <v>187</v>
       </c>
       <c r="F23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -5165,20 +5183,20 @@
         <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E24" t="s">
         <v>187</v>
       </c>
       <c r="F24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -5189,20 +5207,20 @@
         <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E25" t="s">
         <v>187</v>
       </c>
       <c r="F25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -5213,20 +5231,20 @@
         <v>188</v>
       </c>
       <c r="D26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E26" t="s">
         <v>187</v>
       </c>
       <c r="F26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -5237,20 +5255,20 @@
         <v>188</v>
       </c>
       <c r="D27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E27" t="s">
         <v>187</v>
       </c>
       <c r="F27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -5261,20 +5279,20 @@
         <v>188</v>
       </c>
       <c r="D28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E28" t="s">
         <v>187</v>
       </c>
       <c r="F28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -5285,20 +5303,20 @@
         <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E29" t="s">
         <v>187</v>
       </c>
       <c r="F29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -5309,20 +5327,20 @@
         <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E30" t="s">
         <v>187</v>
       </c>
       <c r="F30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -5333,20 +5351,20 @@
         <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E31" t="s">
         <v>187</v>
       </c>
       <c r="F31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -5357,20 +5375,20 @@
         <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E32" t="s">
         <v>187</v>
       </c>
       <c r="F32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -5381,20 +5399,20 @@
         <v>188</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E33" t="s">
         <v>187</v>
       </c>
       <c r="F33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -5405,20 +5423,20 @@
         <v>188</v>
       </c>
       <c r="D34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E34" t="s">
         <v>187</v>
       </c>
       <c r="F34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -5429,20 +5447,20 @@
         <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E35" t="s">
         <v>187</v>
       </c>
       <c r="F35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -5453,20 +5471,20 @@
         <v>188</v>
       </c>
       <c r="D36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E36" t="s">
         <v>187</v>
       </c>
       <c r="F36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -5477,20 +5495,20 @@
         <v>188</v>
       </c>
       <c r="D37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E37" t="s">
         <v>187</v>
       </c>
       <c r="F37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -5501,20 +5519,20 @@
         <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E38" t="s">
         <v>187</v>
       </c>
       <c r="F38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -5525,20 +5543,20 @@
         <v>188</v>
       </c>
       <c r="D39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E39" t="s">
         <v>187</v>
       </c>
       <c r="F39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -5549,20 +5567,20 @@
         <v>188</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E40" t="s">
         <v>187</v>
       </c>
       <c r="F40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -5573,20 +5591,20 @@
         <v>188</v>
       </c>
       <c r="D41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E41" t="s">
         <v>187</v>
       </c>
       <c r="F41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -5597,20 +5615,20 @@
         <v>188</v>
       </c>
       <c r="D42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E42" t="s">
         <v>187</v>
       </c>
       <c r="F42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A6</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -5621,20 +5639,20 @@
         <v>188</v>
       </c>
       <c r="D43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E43" t="s">
         <v>187</v>
       </c>
       <c r="F43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -5645,20 +5663,20 @@
         <v>188</v>
       </c>
       <c r="D44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E44" t="s">
         <v>187</v>
       </c>
       <c r="F44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C6</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -5669,20 +5687,20 @@
         <v>188</v>
       </c>
       <c r="D45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E45" t="s">
         <v>187</v>
       </c>
       <c r="F45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -5693,20 +5711,20 @@
         <v>188</v>
       </c>
       <c r="D46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E46" t="s">
         <v>187</v>
       </c>
       <c r="F46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E6</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -5717,20 +5735,20 @@
         <v>188</v>
       </c>
       <c r="D47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E47" t="s">
         <v>187</v>
       </c>
       <c r="F47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F6</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -5741,20 +5759,20 @@
         <v>188</v>
       </c>
       <c r="D48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E48" t="s">
         <v>187</v>
       </c>
       <c r="F48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G6</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -5765,20 +5783,20 @@
         <v>188</v>
       </c>
       <c r="D49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E49" t="s">
         <v>187</v>
       </c>
       <c r="F49" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H6</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -5789,20 +5807,20 @@
         <v>188</v>
       </c>
       <c r="D50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E50" t="s">
         <v>187</v>
       </c>
       <c r="F50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -5813,20 +5831,20 @@
         <v>188</v>
       </c>
       <c r="D51" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E51" t="s">
         <v>187</v>
       </c>
       <c r="F51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B7</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -5837,20 +5855,20 @@
         <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E52" t="s">
         <v>187</v>
       </c>
       <c r="F52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C7</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -5861,20 +5879,20 @@
         <v>188</v>
       </c>
       <c r="D53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E53" t="s">
         <v>187</v>
       </c>
       <c r="F53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D7</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -5885,20 +5903,20 @@
         <v>188</v>
       </c>
       <c r="D54" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E54" t="s">
         <v>187</v>
       </c>
       <c r="F54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E7</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -5909,20 +5927,20 @@
         <v>188</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E55" t="s">
         <v>187</v>
       </c>
       <c r="F55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F7</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -5933,20 +5951,20 @@
         <v>188</v>
       </c>
       <c r="D56" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E56" t="s">
         <v>187</v>
       </c>
       <c r="F56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G7</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>83</v>
       </c>
@@ -5957,20 +5975,20 @@
         <v>188</v>
       </c>
       <c r="D57" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E57" t="s">
         <v>187</v>
       </c>
       <c r="F57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H7</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -5981,20 +5999,20 @@
         <v>188</v>
       </c>
       <c r="D58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E58" t="s">
         <v>187</v>
       </c>
       <c r="F58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -6005,20 +6023,20 @@
         <v>188</v>
       </c>
       <c r="D59" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E59" t="s">
         <v>187</v>
       </c>
       <c r="F59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01B8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -6029,20 +6047,20 @@
         <v>188</v>
       </c>
       <c r="D60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E60" t="s">
         <v>187</v>
       </c>
       <c r="F60" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01C8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -6053,20 +6071,20 @@
         <v>188</v>
       </c>
       <c r="D61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E61" t="s">
         <v>187</v>
       </c>
       <c r="F61" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01D8</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -6077,20 +6095,20 @@
         <v>188</v>
       </c>
       <c r="D62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E62" t="s">
         <v>187</v>
       </c>
       <c r="F62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01E8</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -6101,20 +6119,20 @@
         <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E63" t="s">
         <v>187</v>
       </c>
       <c r="F63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01F8</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -6125,20 +6143,20 @@
         <v>188</v>
       </c>
       <c r="D64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E64" t="s">
         <v>187</v>
       </c>
       <c r="F64" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01G8</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -6149,20 +6167,20 @@
         <v>188</v>
       </c>
       <c r="D65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E65" t="s">
         <v>187</v>
       </c>
       <c r="F65" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01H8</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>83</v>
       </c>
@@ -6173,20 +6191,20 @@
         <v>188</v>
       </c>
       <c r="D66" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E66" t="s">
         <v>187</v>
       </c>
       <c r="F66" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
         <v>GEP00006_01A9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>83</v>
       </c>
@@ -6197,20 +6215,20 @@
         <v>188</v>
       </c>
       <c r="D67" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E67" t="s">
         <v>187</v>
       </c>
       <c r="F67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" ref="G67:G97" si="1">CONCATENATE(A67,B67)</f>
         <v>GEP00006_01B9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -6221,20 +6239,20 @@
         <v>188</v>
       </c>
       <c r="D68" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E68" t="s">
         <v>187</v>
       </c>
       <c r="F68" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01C9</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -6245,20 +6263,20 @@
         <v>188</v>
       </c>
       <c r="D69" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E69" t="s">
         <v>187</v>
       </c>
       <c r="F69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01D9</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -6269,20 +6287,20 @@
         <v>188</v>
       </c>
       <c r="D70" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E70" t="s">
         <v>187</v>
       </c>
       <c r="F70" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01E9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -6293,20 +6311,20 @@
         <v>188</v>
       </c>
       <c r="D71" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E71" t="s">
         <v>187</v>
       </c>
       <c r="F71" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01F9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -6317,20 +6335,20 @@
         <v>188</v>
       </c>
       <c r="D72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E72" t="s">
         <v>187</v>
       </c>
       <c r="F72" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01G9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>83</v>
       </c>
@@ -6341,20 +6359,20 @@
         <v>188</v>
       </c>
       <c r="D73" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E73" t="s">
         <v>187</v>
       </c>
       <c r="F73" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01H9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -6365,20 +6383,20 @@
         <v>188</v>
       </c>
       <c r="D74" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E74" t="s">
         <v>187</v>
       </c>
       <c r="F74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01A10</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -6389,20 +6407,20 @@
         <v>188</v>
       </c>
       <c r="D75" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E75" t="s">
         <v>187</v>
       </c>
       <c r="F75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01B10</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -6413,20 +6431,20 @@
         <v>188</v>
       </c>
       <c r="D76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E76" t="s">
         <v>187</v>
       </c>
       <c r="F76" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01C10</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -6437,20 +6455,20 @@
         <v>188</v>
       </c>
       <c r="D77" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E77" t="s">
         <v>187</v>
       </c>
       <c r="F77" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01D10</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -6461,20 +6479,20 @@
         <v>188</v>
       </c>
       <c r="D78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E78" t="s">
         <v>187</v>
       </c>
       <c r="F78" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01E10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -6485,20 +6503,20 @@
         <v>188</v>
       </c>
       <c r="D79" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E79" t="s">
         <v>187</v>
       </c>
       <c r="F79" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01F10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -6509,20 +6527,20 @@
         <v>188</v>
       </c>
       <c r="D80" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E80" t="s">
         <v>187</v>
       </c>
       <c r="F80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01G10</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -6533,20 +6551,20 @@
         <v>188</v>
       </c>
       <c r="D81" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E81" t="s">
         <v>187</v>
       </c>
       <c r="F81" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01H10</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -6557,20 +6575,20 @@
         <v>188</v>
       </c>
       <c r="D82" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E82" t="s">
         <v>187</v>
       </c>
       <c r="F82" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01A11</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -6581,20 +6599,20 @@
         <v>188</v>
       </c>
       <c r="D83" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E83" t="s">
         <v>187</v>
       </c>
       <c r="F83" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01B11</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -6605,20 +6623,20 @@
         <v>188</v>
       </c>
       <c r="D84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E84" t="s">
         <v>187</v>
       </c>
       <c r="F84" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01C11</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -6629,20 +6647,20 @@
         <v>188</v>
       </c>
       <c r="D85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E85" t="s">
         <v>187</v>
       </c>
       <c r="F85" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01D11</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -6653,20 +6671,20 @@
         <v>188</v>
       </c>
       <c r="D86" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E86" t="s">
         <v>187</v>
       </c>
       <c r="F86" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01E11</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -6677,20 +6695,20 @@
         <v>188</v>
       </c>
       <c r="D87" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E87" t="s">
         <v>187</v>
       </c>
       <c r="F87" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01F11</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -6701,20 +6719,20 @@
         <v>188</v>
       </c>
       <c r="D88" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E88" t="s">
         <v>187</v>
       </c>
       <c r="F88" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01G11</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>83</v>
       </c>
@@ -6725,20 +6743,20 @@
         <v>188</v>
       </c>
       <c r="D89" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E89" t="s">
         <v>187</v>
       </c>
       <c r="F89" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01H11</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -6749,20 +6767,20 @@
         <v>188</v>
       </c>
       <c r="D90" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E90" t="s">
         <v>187</v>
       </c>
       <c r="F90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01A12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>83</v>
       </c>
@@ -6773,20 +6791,20 @@
         <v>188</v>
       </c>
       <c r="D91" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E91" t="s">
         <v>187</v>
       </c>
       <c r="F91" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01B12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>83</v>
       </c>
@@ -6797,20 +6815,20 @@
         <v>188</v>
       </c>
       <c r="D92" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E92" t="s">
         <v>187</v>
       </c>
       <c r="F92" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01C12</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>83</v>
       </c>
@@ -6821,20 +6839,20 @@
         <v>188</v>
       </c>
       <c r="D93" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E93" t="s">
         <v>187</v>
       </c>
       <c r="F93" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01D12</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>83</v>
       </c>
@@ -6845,20 +6863,20 @@
         <v>188</v>
       </c>
       <c r="D94" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E94" t="s">
         <v>187</v>
       </c>
       <c r="F94" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01E12</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>83</v>
       </c>
@@ -6869,20 +6887,20 @@
         <v>188</v>
       </c>
       <c r="D95" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E95" t="s">
         <v>187</v>
       </c>
       <c r="F95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01F12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>83</v>
       </c>
@@ -6893,20 +6911,20 @@
         <v>188</v>
       </c>
       <c r="D96" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E96" t="s">
         <v>187</v>
       </c>
       <c r="F96" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
         <v>GEP00006_01G12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>83</v>
       </c>
@@ -6917,13 +6935,13 @@
         <v>188</v>
       </c>
       <c r="D97" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E97" t="s">
         <v>187</v>
       </c>
       <c r="F97" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="1"/>
@@ -6937,5 +6955,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>